<commit_message>
New concepts allowed even if name alrady exists in imported ontologies
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/francesca_l_bleken_sintef_no/Documents/Skrivebord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4AA229-0711-4128-97D8-805D85E67D3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5258C8-0C34-4F83-AFCF-0D8473A3DA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37230" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="139">
   <si>
     <t>Metadata name</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Perceptual</t>
   </si>
   <si>
-    <t>Data starts on row 4, Test parent from imported ontology</t>
-  </si>
-  <si>
     <t>SpatioTemporalPattern</t>
   </si>
   <si>
@@ -356,12 +353,6 @@
     <t>Test invalid parent</t>
   </si>
   <si>
-    <t>Test adding concept that already exists in and imported ontology)</t>
-  </si>
-  <si>
-    <t>Test defining same concept twice in the same excel sheet</t>
-  </si>
-  <si>
     <t>SpecialMolecule</t>
   </si>
   <si>
@@ -441,13 +432,28 @@
   </si>
   <si>
     <t>Check that prefix is set to subimport (ontology.ttl)</t>
+  </si>
+  <si>
+    <t>Data starts on row 4</t>
+  </si>
+  <si>
+    <t>Test parent from imported ontology</t>
+  </si>
+  <si>
+    <t>Test defining same concept twice in the same excel sheet, this is not allowed.</t>
+  </si>
+  <si>
+    <t>Test adding concept that already exists in and imported ontology, this should be added with a warning.</t>
+  </si>
+  <si>
+    <t>emmo:Atom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -478,6 +484,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -546,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -584,11 +603,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -979,14 +1000,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="120.140625" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="120.1796875" customWidth="1"/>
+    <col min="3" max="3" width="64.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1027,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1036,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1045,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1033,19 +1054,19 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1083,31 +1104,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
     </row>
   </sheetData>
@@ -1121,69 +1142,69 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="120.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="120.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1199,46 +1220,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" customWidth="1"/>
+    <col min="4" max="4" width="43.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="33.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="69.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
-      <c r="J1" t="s">
+      <c r="J1" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
@@ -1298,8 +1319,11 @@
       <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1313,7 +1337,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1327,18 +1351,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1352,224 +1376,227 @@
         <v>57</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
       </c>
       <c r="I11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>74</v>
       </c>
-      <c r="J12" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>79</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>80</v>
       </c>
-      <c r="J13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="J14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" t="s">
         <v>84</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>85</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>86</v>
       </c>
-      <c r="I15" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>57</v>
       </c>
       <c r="J16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>91</v>
       </c>
-      <c r="J17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" t="s">
         <v>93</v>
       </c>
-      <c r="G18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" t="s">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
+      <c r="J20" t="s">
         <v>97</v>
       </c>
-      <c r="J20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="J22" t="s">
         <v>100</v>
       </c>
-      <c r="J22" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>102</v>
+      <c r="G23" t="s">
+        <v>138</v>
       </c>
       <c r="J23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1582,63 +1609,63 @@
       </c>
       <c r="H24" s="8"/>
       <c r="J24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="G25" t="s">
         <v>110</v>
       </c>
-      <c r="C25" t="s">
+      <c r="I25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>114</v>
       </c>
-      <c r="J25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
       <c r="G26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" t="s">
         <v>133</v>
-      </c>
-      <c r="J28" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1674,7 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1657,11 +1684,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1703,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1691,7 +1718,7 @@
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
New concepts allowed even if name alrady exists in imported ontologies (#504)
* New concepts allowed even if name already exists in imported ontologies
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/francesca_l_bleken_sintef_no/Documents/Skrivebord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4AA229-0711-4128-97D8-805D85E67D3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5258C8-0C34-4F83-AFCF-0D8473A3DA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37230" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="139">
   <si>
     <t>Metadata name</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Perceptual</t>
   </si>
   <si>
-    <t>Data starts on row 4, Test parent from imported ontology</t>
-  </si>
-  <si>
     <t>SpatioTemporalPattern</t>
   </si>
   <si>
@@ -356,12 +353,6 @@
     <t>Test invalid parent</t>
   </si>
   <si>
-    <t>Test adding concept that already exists in and imported ontology)</t>
-  </si>
-  <si>
-    <t>Test defining same concept twice in the same excel sheet</t>
-  </si>
-  <si>
     <t>SpecialMolecule</t>
   </si>
   <si>
@@ -441,13 +432,28 @@
   </si>
   <si>
     <t>Check that prefix is set to subimport (ontology.ttl)</t>
+  </si>
+  <si>
+    <t>Data starts on row 4</t>
+  </si>
+  <si>
+    <t>Test parent from imported ontology</t>
+  </si>
+  <si>
+    <t>Test defining same concept twice in the same excel sheet, this is not allowed.</t>
+  </si>
+  <si>
+    <t>Test adding concept that already exists in and imported ontology, this should be added with a warning.</t>
+  </si>
+  <si>
+    <t>emmo:Atom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -478,6 +484,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -546,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -584,11 +603,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -979,14 +1000,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="120.140625" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="120.1796875" customWidth="1"/>
+    <col min="3" max="3" width="64.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1027,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1036,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1045,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1033,19 +1054,19 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1083,31 +1104,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="9"/>
     </row>
   </sheetData>
@@ -1121,69 +1142,69 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="120.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="120.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1199,46 +1220,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" customWidth="1"/>
+    <col min="4" max="4" width="43.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="33.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="69.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
-      <c r="J1" t="s">
+      <c r="J1" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
@@ -1298,8 +1319,11 @@
       <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1313,7 +1337,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1327,18 +1351,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1352,224 +1376,227 @@
         <v>57</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" t="s">
         <v>64</v>
       </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
       </c>
       <c r="I11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>74</v>
       </c>
-      <c r="J12" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>79</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>80</v>
       </c>
-      <c r="J13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="J14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" t="s">
         <v>84</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>85</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>86</v>
       </c>
-      <c r="I15" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>57</v>
       </c>
       <c r="J16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>91</v>
       </c>
-      <c r="J17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" t="s">
         <v>93</v>
       </c>
-      <c r="G18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" t="s">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
+      <c r="J20" t="s">
         <v>97</v>
       </c>
-      <c r="J20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="J22" t="s">
         <v>100</v>
       </c>
-      <c r="J22" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>102</v>
+      <c r="G23" t="s">
+        <v>138</v>
       </c>
       <c r="J23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1582,63 +1609,63 @@
       </c>
       <c r="H24" s="8"/>
       <c r="J24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="G25" t="s">
         <v>110</v>
       </c>
-      <c r="C25" t="s">
+      <c r="I25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>114</v>
       </c>
-      <c r="J25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
       <c r="G26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" t="s">
         <v>133</v>
-      </c>
-      <c r="J28" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1674,7 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1657,11 +1684,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1703,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1691,7 +1718,7 @@
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Data properties, object properties and annotation properties in Excelparser
If these sheets do not exist in the excel workbook they will not be considered.

Other annotations have been added.
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCAA9E7-41E5-49ED-9441-8E44E4E6ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD26EC8-91F9-422D-B10D-21F6CD829724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1110" windowWidth="30210" windowHeight="15600" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="1500" windowWidth="38700" windowHeight="15525" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="169">
   <si>
     <t>Metadata name</t>
   </si>
@@ -507,6 +507,36 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>Boundary; Material</t>
+  </si>
+  <si>
+    <t>SpecialBoundary</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"</t>
+  </si>
+  <si>
+    <t>subAnnotation</t>
+  </si>
+  <si>
+    <t>hasSubBoundaryPart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary </t>
+  </si>
+  <si>
+    <t>hasPrimeNumberData</t>
+  </si>
+  <si>
+    <t>SuperSpecialBoundary</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaEntry="A very secure source"; subAnnotation="Another thing"</t>
+  </si>
+  <si>
+    <t>A special boundary.</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1321,7 @@
     <col min="3" max="3" width="41.5703125" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
@@ -1728,6 +1758,31 @@
         <v>132</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
@@ -1740,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1916,21 @@
         <v>90</v>
       </c>
       <c r="K4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" t="s">
         <v>90</v>
+      </c>
+      <c r="K5" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1876,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1959,7 @@
     <col min="4" max="4" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1961,6 +2030,14 @@
       </c>
       <c r="G4" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1975,10 +2052,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,6 +2163,20 @@
         <v>158</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Support for data, object and annotation properties
Moved adding of concepts to help_function _add_entities, which can be used to add entities fo type owlread2.Thing/ObjectProperty/AnnotationProperty/DataProperty. _add_entities adds annotation properties, but not relations for classes or ranges and domains for properties

Data properties, object properties and annotation properties should be provided in separate sheets called AnnotationProperties, DataProperties, ObjectProperties
If these sheets do not exist in the excel workbook they will not be considered. The same if the sheets exist, but do not have prefLabels.

An extra column for OtherAnnotations has been added and it is now read correctly.

The dictionary with errors is now returned with separate keys for the different properties and classes.
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5258C8-0C34-4F83-AFCF-0D8473A3DA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD26EC8-91F9-422D-B10D-21F6CD829724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="1500" windowWidth="38700" windowHeight="15525" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="169">
   <si>
     <t>Metadata name</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Atom</t>
   </si>
   <si>
-    <t>Object</t>
-  </si>
-  <si>
     <t>SubSubgrainBoundary</t>
   </si>
   <si>
@@ -447,6 +444,99 @@
   </si>
   <si>
     <t>emmo:Atom</t>
+  </si>
+  <si>
+    <t>subPropertyOf</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>inverseOf</t>
+  </si>
+  <si>
+    <t>parent properties(s), separate with ";"</t>
+  </si>
+  <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>Ranges</t>
+  </si>
+  <si>
+    <t>Separate domains with ";"</t>
+  </si>
+  <si>
+    <t>inverse concept</t>
+  </si>
+  <si>
+    <t>disjointWith</t>
+  </si>
+  <si>
+    <t>Separatete ranges with ";"</t>
+  </si>
+  <si>
+    <t>hasPart</t>
+  </si>
+  <si>
+    <t>has a part that is a boundary</t>
+  </si>
+  <si>
+    <t>This definition is humbug</t>
+  </si>
+  <si>
+    <t>hasBoundaryPart</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry</t>
+  </si>
+  <si>
+    <t>Where to find the entry in the "book of boundaries"</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>hasIntegerData</t>
+  </si>
+  <si>
+    <t>hasNumericalData</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Boundary; Material</t>
+  </si>
+  <si>
+    <t>SpecialBoundary</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"</t>
+  </si>
+  <si>
+    <t>subAnnotation</t>
+  </si>
+  <si>
+    <t>hasSubBoundaryPart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary </t>
+  </si>
+  <si>
+    <t>hasPrimeNumberData</t>
+  </si>
+  <si>
+    <t>SuperSpecialBoundary</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaEntry="A very secure source"; subAnnotation="Another thing"</t>
+  </si>
+  <si>
+    <t>A special boundary.</t>
   </si>
 </sst>
 </file>
@@ -1000,14 +1090,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="120.1796875" customWidth="1"/>
-    <col min="3" max="3" width="64.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="120.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1117,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1126,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1135,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1054,19 +1144,19 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1096,7 +1186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1104,31 +1194,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
     </row>
   </sheetData>
@@ -1145,64 +1235,64 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="120.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" customWidth="1"/>
+    <col min="1" max="1" width="120.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>92</v>
       </c>
@@ -1218,30 +1308,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="41.54296875" customWidth="1"/>
-    <col min="4" max="4" width="43.81640625" customWidth="1"/>
-    <col min="5" max="5" width="29.54296875" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" customWidth="1"/>
-    <col min="7" max="7" width="33.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="69.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="21.54296875" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
@@ -1291,7 +1381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
@@ -1320,10 +1410,10 @@
         <v>45</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1337,7 +1427,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1351,18 +1441,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1377,10 +1467,10 @@
       </c>
       <c r="H7" s="8"/>
       <c r="J7" s="20" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1398,7 +1488,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1409,14 +1499,14 @@
         <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1431,7 +1521,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1448,7 +1538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1462,7 +1552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -1482,13 +1572,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="J14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1505,7 +1595,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -1519,7 +1609,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -1533,7 +1623,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1547,7 +1637,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -1558,7 +1648,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>96</v>
       </c>
@@ -1566,7 +1656,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1577,7 +1667,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1585,18 +1675,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>101</v>
       </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1609,63 +1699,88 @@
       </c>
       <c r="H24" s="8"/>
       <c r="J24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
         <v>107</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>108</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>109</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>110</v>
       </c>
-      <c r="I25" t="s">
-        <v>111</v>
-      </c>
       <c r="J25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" t="s">
+        <v>129</v>
+      </c>
+      <c r="J28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" t="s">
-        <v>115</v>
-      </c>
-      <c r="I26" t="s">
-        <v>116</v>
-      </c>
-      <c r="J26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>122</v>
-      </c>
-      <c r="G27" t="s">
-        <v>123</v>
-      </c>
-      <c r="J27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" t="s">
-        <v>130</v>
-      </c>
-      <c r="J28" t="s">
-        <v>133</v>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1680,18 +1795,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="47" customWidth="1"/>
+    <col min="10" max="11" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>102</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1699,12 +1945,106 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1712,14 +2052,136 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated excelparser to use emmo1.0.0-beta4, patch and excelparser OK.
It was needed to udate the search for annotation property seach with
getattr for ThingClass
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\flb\projects\Team4.0\EMMOntoPy\tests\test_excelparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD26EC8-91F9-422D-B10D-21F6CD829724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A191A439-EA3D-42C4-BD9B-0879305C030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="1500" windowWidth="38700" windowHeight="15525" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-2685" windowWidth="38640" windowHeight="23790" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Resolvable URL or path to imported ontologies (one per line )</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta/emmo-inferred-chemistry2.ttl</t>
-  </si>
-  <si>
     <t>Concept</t>
   </si>
   <si>
@@ -194,15 +191,9 @@
     <t>Test of undefined parent</t>
   </si>
   <si>
-    <t>Pattern</t>
-  </si>
-  <si>
     <t>everything that can be perceived or measured</t>
   </si>
   <si>
-    <t>a pattern is defined from a contrast; this definition is much broader than definition of pattern such as "the regular and repeated way in which something happens or is"</t>
-  </si>
-  <si>
     <t>Perceptual</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
     <t>Test of undefined parent without elucidation</t>
   </si>
   <si>
-    <t>SpatioTemporal Pattern</t>
-  </si>
-  <si>
     <t>Test invalid parent</t>
   </si>
   <si>
@@ -500,9 +488,6 @@
     <t>hasIntegerData</t>
   </si>
   <si>
-    <t>hasNumericalData</t>
-  </si>
-  <si>
     <t>Numerical</t>
   </si>
   <si>
@@ -533,10 +518,25 @@
     <t>SuperSpecialBoundary</t>
   </si>
   <si>
-    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaEntry="A very secure source"; subAnnotation="Another thing"</t>
-  </si>
-  <si>
     <t>A special boundary.</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta4/emmo-inferred.ttl</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaReference="http at wikipedia"; subAnnotation="Another thing"</t>
+  </si>
+  <si>
+    <t>hasNumericalValue</t>
+  </si>
+  <si>
+    <t>SpecialPattern</t>
+  </si>
+  <si>
+    <t>SpatioTemporal SpecialPattern</t>
+  </si>
+  <si>
+    <t>a pattern is defined from a contrast; this definition is much broader than definition of pattern such as "the regular and repeated way in which something happens or is"; note that this is changed from pattern as Pattern is from emmo-beta4 an altLabel for Data</t>
   </si>
 </sst>
 </file>
@@ -658,19 +658,19 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -693,17 +693,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,7 +788,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1090,7 +1090,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="120.140625" customWidth="1"/>
@@ -1231,11 +1231,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="120.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -1247,10 +1247,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1258,43 +1258,43 @@
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1310,11 +1310,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -1333,11 +1333,11 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1346,314 +1346,314 @@
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
       <c r="J1" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>45</v>
-      </c>
       <c r="J3" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>48</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
       </c>
       <c r="H7" s="8"/>
       <c r="J7" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="I13" t="s">
         <v>76</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J13" t="s">
         <v>77</v>
-      </c>
-      <c r="G13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="J14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G15" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="I15" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" t="s">
         <v>90</v>
-      </c>
-      <c r="J18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1661,126 +1661,126 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" s="8"/>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H24" s="8"/>
       <c r="J24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" t="s">
         <v>106</v>
       </c>
-      <c r="C25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" t="s">
-        <v>110</v>
-      </c>
       <c r="J25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" t="s">
         <v>128</v>
-      </c>
-      <c r="G28" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +1801,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1816,11 +1816,11 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1833,104 +1833,104 @@
     </row>
     <row r="2" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>142</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1948,10 +1948,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -1964,11 +1964,11 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1977,67 +1977,67 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2055,10 +2055,10 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -2073,11 +2073,11 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -2089,92 +2089,92 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>142</v>
-      </c>
       <c r="J2" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to comply with owlready2>0.41 (#639)
* Update to comply with owlready2>0.41 which returns a owlready2.locstr
instead of str


* Updated excelparser to use emmo1.0.0-beta4, patch and excelparser OK.

* _getattr monkey patch so that ThingClass annotations can be directly accessed.

* Added some get_by_albel_tests that codecov is complaining about.

* Added wu-palmer test in test_generations
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\flb\projects\Team4.0\EMMOntoPy\tests\test_excelparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD26EC8-91F9-422D-B10D-21F6CD829724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A191A439-EA3D-42C4-BD9B-0879305C030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="1500" windowWidth="38700" windowHeight="15525" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-2685" windowWidth="38640" windowHeight="23790" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Resolvable URL or path to imported ontologies (one per line )</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta/emmo-inferred-chemistry2.ttl</t>
-  </si>
-  <si>
     <t>Concept</t>
   </si>
   <si>
@@ -194,15 +191,9 @@
     <t>Test of undefined parent</t>
   </si>
   <si>
-    <t>Pattern</t>
-  </si>
-  <si>
     <t>everything that can be perceived or measured</t>
   </si>
   <si>
-    <t>a pattern is defined from a contrast; this definition is much broader than definition of pattern such as "the regular and repeated way in which something happens or is"</t>
-  </si>
-  <si>
     <t>Perceptual</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
     <t>Test of undefined parent without elucidation</t>
   </si>
   <si>
-    <t>SpatioTemporal Pattern</t>
-  </si>
-  <si>
     <t>Test invalid parent</t>
   </si>
   <si>
@@ -500,9 +488,6 @@
     <t>hasIntegerData</t>
   </si>
   <si>
-    <t>hasNumericalData</t>
-  </si>
-  <si>
     <t>Numerical</t>
   </si>
   <si>
@@ -533,10 +518,25 @@
     <t>SuperSpecialBoundary</t>
   </si>
   <si>
-    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaEntry="A very secure source"; subAnnotation="Another thing"</t>
-  </si>
-  <si>
     <t>A special boundary.</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta4/emmo-inferred.ttl</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaReference="http at wikipedia"; subAnnotation="Another thing"</t>
+  </si>
+  <si>
+    <t>hasNumericalValue</t>
+  </si>
+  <si>
+    <t>SpecialPattern</t>
+  </si>
+  <si>
+    <t>SpatioTemporal SpecialPattern</t>
+  </si>
+  <si>
+    <t>a pattern is defined from a contrast; this definition is much broader than definition of pattern such as "the regular and repeated way in which something happens or is"; note that this is changed from pattern as Pattern is from emmo-beta4 an altLabel for Data</t>
   </si>
 </sst>
 </file>
@@ -658,19 +658,19 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -693,17 +693,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,7 +788,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1090,7 +1090,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="120.140625" customWidth="1"/>
@@ -1231,11 +1231,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="120.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -1247,10 +1247,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1258,43 +1258,43 @@
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1310,11 +1310,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -1333,11 +1333,11 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1346,314 +1346,314 @@
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
       <c r="J1" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>45</v>
-      </c>
       <c r="J3" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>48</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
       </c>
       <c r="H7" s="8"/>
       <c r="J7" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="I13" t="s">
         <v>76</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J13" t="s">
         <v>77</v>
-      </c>
-      <c r="G13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="J14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G15" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="I15" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" t="s">
         <v>90</v>
-      </c>
-      <c r="J18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1661,126 +1661,126 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" s="8"/>
       <c r="G24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H24" s="8"/>
       <c r="J24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" t="s">
         <v>106</v>
       </c>
-      <c r="C25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" t="s">
-        <v>110</v>
-      </c>
       <c r="J25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" t="s">
         <v>128</v>
-      </c>
-      <c r="G28" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +1801,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1816,11 +1816,11 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1833,104 +1833,104 @@
     </row>
     <row r="2" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>142</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1948,10 +1948,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -1964,11 +1964,11 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1977,67 +1977,67 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2055,10 +2055,10 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -2073,11 +2073,11 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -2089,92 +2089,92 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>142</v>
-      </c>
       <c r="J2" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added possibility for = in extra annotations defined in excelparser
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\flb\projects\Team4.0\EMMOntoPy\tests\test_excelparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A191A439-EA3D-42C4-BD9B-0879305C030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C537C49F-0E7D-4731-A0E1-8F36F2FB8AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-2685" windowWidth="38640" windowHeight="23790" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="345" windowWidth="27360" windowHeight="15600" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="AnnotationProperties" sheetId="5" r:id="rId5"/>
     <sheet name="DataProperties" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="171">
   <si>
     <t>Metadata name</t>
   </si>
@@ -500,9 +500,6 @@
     <t>SpecialBoundary</t>
   </si>
   <si>
-    <t>bookOfBoundariesEntry="A text about this type of boundary"</t>
-  </si>
-  <si>
     <t>subAnnotation</t>
   </si>
   <si>
@@ -537,6 +534,15 @@
   </si>
   <si>
     <t>a pattern is defined from a contrast; this definition is much broader than definition of pattern such as "the regular and repeated way in which something happens or is"; note that this is changed from pattern as Pattern is from emmo-beta4 an altLabel for Data</t>
+  </si>
+  <si>
+    <t>bookOfBoundariesEntry="A text about this type of=boundary"</t>
+  </si>
+  <si>
+    <t>Check extra annotation, with an '=' in the string</t>
+  </si>
+  <si>
+    <t>Check adding more than one annotation</t>
   </si>
 </sst>
 </file>
@@ -788,9 +794,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -828,7 +834,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -934,7 +940,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1076,7 +1082,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1231,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1269,7 +1275,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
         <v>108</v>
@@ -1310,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,13 +1460,13 @@
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
@@ -1481,7 +1487,7 @@
         <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
@@ -1499,7 +1505,7 @@
         <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
@@ -1532,7 +1538,7 @@
         <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I11" t="s">
         <v>68</v>
@@ -1688,7 +1694,7 @@
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>53</v>
@@ -1763,24 +1769,30 @@
         <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F29" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="G29" t="s">
         <v>87</v>
       </c>
+      <c r="J29" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G30" t="s">
         <v>87</v>
+      </c>
+      <c r="J30" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1933,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
         <v>147</v>
@@ -1930,7 +1942,7 @@
         <v>87</v>
       </c>
       <c r="K5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2034,7 +2046,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
         <v>148</v>
@@ -2154,7 +2166,7 @@
         <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I4" t="s">
         <v>152</v>
@@ -2165,7 +2177,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G5" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Updated excelparser-tests with emmo-1.0.0
</commit_message>
<xml_diff>
--- a/tests/test_excelparser/onto.xlsx
+++ b/tests/test_excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\flb\projects\Team4.0\EMMOntoPy\tests\test_excelparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C537C49F-0E7D-4731-A0E1-8F36F2FB8AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F62E00-332A-4644-BCFE-58C676F44153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="345" windowWidth="27360" windowHeight="15600" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48090" yWindow="-6765" windowWidth="38700" windowHeight="15345" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -518,9 +518,6 @@
     <t>A special boundary.</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/emmo-repo/emmo-repo.github.io/master/versions/1.0.0-beta4/emmo-inferred.ttl</t>
-  </si>
-  <si>
     <t>bookOfBoundariesEntry="A text about this type of boundary"; wikipediaReference="http at wikipedia"; subAnnotation="Another thing"</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>Check adding more than one annotation</t>
+  </si>
+  <si>
+    <t>https://w3id.org/emmo/inferred</t>
   </si>
 </sst>
 </file>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
         <v>108</v>
@@ -1305,7 +1305,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{4AE6D9F9-5AA3-467D-A245-2C36C0027930}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{33CC3B70-5CD5-4594-B662-DF452B3A2B7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1316,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="E4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
@@ -1487,7 +1487,7 @@
         <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H8" s="8"/>
       <c r="J8" t="s">
@@ -1505,7 +1505,7 @@
         <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H9" s="8"/>
       <c r="J9" t="s">
@@ -1538,7 +1538,7 @@
         <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I11" t="s">
         <v>68</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>53</v>
@@ -1772,13 +1772,13 @@
         <v>161</v>
       </c>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G29" t="s">
         <v>87</v>
       </c>
       <c r="J29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1786,13 +1786,13 @@
         <v>160</v>
       </c>
       <c r="F30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G30" t="s">
         <v>87</v>
       </c>
       <c r="J30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +2166,7 @@
         <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I4" t="s">
         <v>152</v>

</xml_diff>